<commit_message>
Progress on generating topology & xyz's
</commit_message>
<xml_diff>
--- a/Final Project/topo_tool.xlsx
+++ b/Final Project/topo_tool.xlsx
@@ -9,15 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="5760" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11496" windowHeight="5760" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Bonds" sheetId="1" r:id="rId1"/>
     <sheet name="Angles" sheetId="2" r:id="rId2"/>
     <sheet name="Dihedrals" sheetId="3" r:id="rId3"/>
     <sheet name="LJ" sheetId="4" r:id="rId4"/>
+    <sheet name="Coords" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="6">
   <si>
     <t>outputFile.write(f"{9*i +</t>
   </si>
@@ -36,6 +38,15 @@
   </si>
   <si>
     <t>outputFile.write(f'{12*i +</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>O</t>
   </si>
 </sst>
 </file>
@@ -359,14 +370,14 @@
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -387,7 +398,7 @@
         <v>outputFile.write(f"{9*i +1} {9*i + 0} 2845.12 1.09 \n' )</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -408,7 +419,7 @@
         <v>outputFile.write(f"{9*i +2} {9*i + 0} 2845.12 1.09 \n' )</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -429,7 +440,7 @@
         <v>outputFile.write(f"{9*i +3} {9*i + 0} 2845.12 1.09 \n' )</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -450,7 +461,7 @@
         <v>outputFile.write(f"{9*i +0} {9*i + 4} 2242.624 1.529 \n' )</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -471,7 +482,7 @@
         <v>outputFile.write(f"{9*i +5} {9*i + 4} 2845.12 1.09 \n' )</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -492,7 +503,7 @@
         <v>outputFile.write(f"{9*i +6} {9*i + 4} 2845.12 1.09 \n' )</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -513,7 +524,7 @@
         <v>outputFile.write(f"{9*i +4} {9*i + 7} 2677.76 1.41 \n' )</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -547,15 +558,15 @@
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="2" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="60.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -579,7 +590,7 @@
         <v>outputFile.write(f'{13*i +1} {13*i + 0} {13*i + 4} 292.88 1.89368 \n' )</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -603,7 +614,7 @@
         <v>outputFile.write(f'{13*i +2} {13*i + 0} {13*i + 4} 292.88 1.89368 \n' )</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -627,7 +638,7 @@
         <v>outputFile.write(f'{13*i +3} {13*i + 0} {13*i + 4} 292.88 1.89368 \n' )</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -651,7 +662,7 @@
         <v>outputFile.write(f'{13*i +3} {13*i + 0} {13*i + 2} 276.144 1.88146 \n' )</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -675,7 +686,7 @@
         <v>outputFile.write(f'{13*i +3} {13*i + 0} {13*i + 1} 276.144 1.88146 \n' )</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -699,7 +710,7 @@
         <v>outputFile.write(f'{13*i +2} {13*i + 0} {13*i + 1} 276.144 1.88146 \n' )</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -723,7 +734,7 @@
         <v>outputFile.write(f'{13*i +5} {13*i + 4} {13*i + 6} 276.144 1.88146 \n' )</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -747,7 +758,7 @@
         <v>outputFile.write(f'{13*i +0} {13*i + 4} {13*i + 6} 313.8 1.93208 \n' )</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -771,7 +782,7 @@
         <v>outputFile.write(f'{13*i +0} {13*i + 4} {13*i + 5} 313.8 1.93208 \n' )</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -795,7 +806,7 @@
         <v>outputFile.write(f'{13*i +0} {13*i + 4} {13*i + 7} 414.4 1.91114 \n' )</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -819,7 +830,7 @@
         <v>outputFile.write(f'{13*i +4} {13*i + 7} {13*i + 8} 460.24 1.89368 \n' )</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -843,7 +854,7 @@
         <v>outputFile.write(f'{13*i +5} {13*i + 4} {13*i + 7} 292.88 1.91114 \n' )</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -880,16 +891,16 @@
       <selection activeCell="J1" sqref="J1:J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="2" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="84.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="84.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -922,7 +933,7 @@
         <v>outputFile.write(f'{12*i +1} {12*i + 0} {12*i + 4} {12*i + 5} 0.6276 1.8828 0 -3.91622 \n' )</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -955,7 +966,7 @@
         <v>outputFile.write(f'{12*i +2} {12*i + 0} {12*i + 4} {12*i + 5} 0.6276 1.8828 0 -3.91622 \n' )</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -988,7 +999,7 @@
         <v>outputFile.write(f'{12*i +3} {12*i + 0} {12*i + 4} {12*i + 5} 0.6276 1.8828 0 -3.91622 \n' )</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1021,7 +1032,7 @@
         <v>outputFile.write(f'{12*i +1} {12*i + 0} {12*i + 4} {12*i + 6} 0.6276 1.8828 0 -3.91622 \n' )</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1054,7 +1065,7 @@
         <v>outputFile.write(f'{12*i +2} {12*i + 0} {12*i + 4} {12*i + 6} 0.6276 1.8828 0 -3.91622 \n' )</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1087,7 +1098,7 @@
         <v>outputFile.write(f'{12*i +3} {12*i + 0} {12*i + 4} {12*i + 6} 0.6276 1.8828 0 -3.91622 \n' )</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1120,7 +1131,7 @@
         <v>outputFile.write(f'{12*i +1} {12*i + 0} {12*i + 4} {12*i + 7} 0.97905 2.93716 0 -3.91622 \n' )</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1153,7 +1164,7 @@
         <v>outputFile.write(f'{12*i +2} {12*i + 0} {12*i + 4} {12*i + 7} 0.97905 2.93716 0 -3.91622 \n' )</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -1186,7 +1197,7 @@
         <v>outputFile.write(f'{12*i +3} {12*i + 0} {12*i + 4} {12*i + 7} 0.97905 2.93716 0 -3.91622 \n' )</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1219,7 +1230,7 @@
         <v>outputFile.write(f'{12*i +0} {12*i + 4} {12*i + 7} {12*i + 8} -0.4431 3.83255 0.72801 -4.11705 \n' )</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -1252,7 +1263,7 @@
         <v>outputFile.write(f'{12*i +5} {12*i + 4} {12*i + 7} {12*i + 8} 0.9414 2.8242 0 -3.7656 \n' )</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -1294,16 +1305,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>3.5</v>
       </c>
@@ -1315,7 +1326,7 @@
         <v>outputFile.write('3.5 0.276144 \n')</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2.5</v>
       </c>
@@ -1327,7 +1338,7 @@
         <v>outputFile.write('2.5 0.12552 \n')</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2.5</v>
       </c>
@@ -1339,7 +1350,7 @@
         <v>outputFile.write('2.5 0.12552 \n')</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2.5</v>
       </c>
@@ -1351,7 +1362,7 @@
         <v>outputFile.write('2.5 0.12552 \n')</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3.5</v>
       </c>
@@ -1363,7 +1374,7 @@
         <v>outputFile.write('3.5 0.276144 \n')</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2.5</v>
       </c>
@@ -1375,7 +1386,7 @@
         <v>outputFile.write('2.5 0.12552 \n')</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2.5</v>
       </c>
@@ -1387,7 +1398,7 @@
         <v>outputFile.write('2.5 0.12552 \n')</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>3.12</v>
       </c>
@@ -1399,7 +1410,7 @@
         <v>outputFile.write('3.12 0.71128 \n')</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0</v>
       </c>
@@ -1411,7 +1422,7 @@
         <v>outputFile.write('0 0 \n')</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>4166</v>
       </c>
@@ -1420,7 +1431,7 @@
         <v>899.85599999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1284</v>
       </c>
@@ -1429,7 +1440,7 @@
         <v>277.34399999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>3488</v>
       </c>
@@ -1438,13 +1449,190 @@
         <v>753.40800000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>228</v>
       </c>
       <c r="B15">
         <f t="shared" si="1"/>
         <v>49.247999999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>0.5</v>
+      </c>
+      <c r="E1" t="str">
+        <f>CONCATENATE("outputFile.write(f'", A1, " {rand[0] + ", B1,"} {rand[1] + ", C1,"} {rand[1] + ", D1,"} \n')" )</f>
+        <v>outputFile.write(f'C {rand[0] + 2} {rand[1] + 2} {rand[1] + 0.5} \n')</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0.2</v>
+      </c>
+      <c r="E2" t="str">
+        <f t="shared" ref="E2:E9" si="0">CONCATENATE("outputFile.write(f'", A2, " {rand[0] + ", B2,"} {rand[1] + ", C2,"} {rand[1] + ", D2,"} \n')" )</f>
+        <v>outputFile.write(f'H {rand[0] + 2} {rand[1] + 1} {rand[1] + 0.2} \n')</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" si="0"/>
+        <v>outputFile.write(f'H {rand[0] + 1} {rand[1] + 2} {rand[1] + 1.1} \n')</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>0.1</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>outputFile.write(f'H {rand[0] + 2} {rand[1] + 3} {rand[1] + 0.1} \n')</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>3.5</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>0.9</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>outputFile.write(f'C {rand[0] + 3.5} {rand[1] + 2} {rand[1] + 0.9} \n')</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>3.5</v>
+      </c>
+      <c r="C6">
+        <v>2.8</v>
+      </c>
+      <c r="D6">
+        <v>1.7</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>outputFile.write(f'H {rand[0] + 3.5} {rand[1] + 2.8} {rand[1] + 1.7} \n')</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>3.5</v>
+      </c>
+      <c r="C7">
+        <v>1.3</v>
+      </c>
+      <c r="D7">
+        <v>1.7</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>outputFile.write(f'H {rand[0] + 3.5} {rand[1] + 1.3} {rand[1] + 1.7} \n')</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>0.4</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="0"/>
+        <v>outputFile.write(f'O {rand[0] + 5} {rand[1] + 2} {rand[1] + 0.4} \n')</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>5.5</v>
+      </c>
+      <c r="C9">
+        <v>2.5</v>
+      </c>
+      <c r="D9">
+        <v>0.2</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="0"/>
+        <v>outputFile.write(f'H {rand[0] + 5.5} {rand[1] + 2.5} {rand[1] + 0.2} \n')</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finish topology & xyz generator
</commit_message>
<xml_diff>
--- a/Final Project/topo_tool.xlsx
+++ b/Final Project/topo_tool.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11496" windowHeight="5760" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9576" windowHeight="2028" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Bonds" sheetId="1" r:id="rId1"/>
@@ -1465,7 +1465,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E9"/>
@@ -1478,17 +1478,17 @@
         <v>3</v>
       </c>
       <c r="B1">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="C1">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D1">
         <v>0.5</v>
       </c>
       <c r="E1" t="str">
-        <f>CONCATENATE("outputFile.write(f'", A1, " {rand[0] + ", B1,"} {rand[1] + ", C1,"} {rand[1] + ", D1,"} \n')" )</f>
-        <v>outputFile.write(f'C {rand[0] + 2} {rand[1] + 2} {rand[1] + 0.5} \n')</v>
+        <f>CONCATENATE("outputFile.write(f'", A1, " {rand[i][0] + ", B1,"} {rand[i][1] + ", C1,"} {rand[i][2] + ", D1,"} \n')" )</f>
+        <v>outputFile.write(f'C {rand[i][0] + -1} {rand[i][1] + -1} {rand[i][2] + 0.5} \n')</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1496,17 +1496,17 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="D2">
         <v>0.2</v>
       </c>
       <c r="E2" t="str">
-        <f t="shared" ref="E2:E9" si="0">CONCATENATE("outputFile.write(f'", A2, " {rand[0] + ", B2,"} {rand[1] + ", C2,"} {rand[1] + ", D2,"} \n')" )</f>
-        <v>outputFile.write(f'H {rand[0] + 2} {rand[1] + 1} {rand[1] + 0.2} \n')</v>
+        <f t="shared" ref="E2:E9" si="0">CONCATENATE("outputFile.write(f'", A2, " {rand[i][0] + ", B2,"} {rand[i][1] + ", C2,"} {rand[i][2] + ", D2,"} \n')" )</f>
+        <v>outputFile.write(f'H {rand[i][0] + -1} {rand[i][1] + -2} {rand[i][2] + 0.2} \n')</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1514,17 +1514,17 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D3">
         <v>1.1000000000000001</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" si="0"/>
-        <v>outputFile.write(f'H {rand[0] + 1} {rand[1] + 2} {rand[1] + 1.1} \n')</v>
+        <v>outputFile.write(f'H {rand[i][0] + -2} {rand[i][1] + -1} {rand[i][2] + 1.1} \n')</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1532,17 +1532,17 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <v>0.1</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
-        <v>outputFile.write(f'H {rand[0] + 2} {rand[1] + 3} {rand[1] + 0.1} \n')</v>
+        <v>outputFile.write(f'H {rand[i][0] + -1} {rand[i][1] + 0} {rand[i][2] + 0.1} \n')</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1550,17 +1550,17 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>3.5</v>
+        <v>0.5</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D5">
         <v>0.9</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
-        <v>outputFile.write(f'C {rand[0] + 3.5} {rand[1] + 2} {rand[1] + 0.9} \n')</v>
+        <v>outputFile.write(f'C {rand[i][0] + 0.5} {rand[i][1] + -1} {rand[i][2] + 0.9} \n')</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1568,17 +1568,17 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>3.5</v>
+        <v>0.5</v>
       </c>
       <c r="C6">
-        <v>2.8</v>
+        <v>-0.20000000000000018</v>
       </c>
       <c r="D6">
         <v>1.7</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
-        <v>outputFile.write(f'H {rand[0] + 3.5} {rand[1] + 2.8} {rand[1] + 1.7} \n')</v>
+        <v>outputFile.write(f'H {rand[i][0] + 0.5} {rand[i][1] + -0.2} {rand[i][2] + 1.7} \n')</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1586,17 +1586,17 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <v>3.5</v>
+        <v>0.5</v>
       </c>
       <c r="C7">
-        <v>1.3</v>
+        <v>-1.7</v>
       </c>
       <c r="D7">
         <v>1.7</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
-        <v>outputFile.write(f'H {rand[0] + 3.5} {rand[1] + 1.3} {rand[1] + 1.7} \n')</v>
+        <v>outputFile.write(f'H {rand[i][0] + 0.5} {rand[i][1] + -1.7} {rand[i][2] + 1.7} \n')</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1604,17 +1604,17 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D8">
         <v>0.4</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
-        <v>outputFile.write(f'O {rand[0] + 5} {rand[1] + 2} {rand[1] + 0.4} \n')</v>
+        <v>outputFile.write(f'O {rand[i][0] + 2} {rand[i][1] + -1} {rand[i][2] + 0.4} \n')</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1622,17 +1622,161 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <v>5.5</v>
+        <v>2.5</v>
       </c>
       <c r="C9">
-        <v>2.5</v>
+        <v>-0.5</v>
       </c>
       <c r="D9">
         <v>0.2</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
-        <v>outputFile.write(f'H {rand[0] + 5.5} {rand[1] + 2.5} {rand[1] + 0.2} \n')</v>
+        <v>outputFile.write(f'H {rand[i][0] + 2.5} {rand[i][1] + -0.5} {rand[i][2] + 0.2} \n')</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <f xml:space="preserve"> A13 - 3</f>
+        <v>-1</v>
+      </c>
+      <c r="E13">
+        <f xml:space="preserve"> B13 - 3</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ref="D14:E21" si="1" xml:space="preserve"> A14 - 3</f>
+        <v>-1</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>-2</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>3.5</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>3.5</v>
+      </c>
+      <c r="B18">
+        <v>2.8</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>-0.20000000000000018</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>3.5</v>
+      </c>
+      <c r="B19">
+        <v>1.3</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>-1.7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>5.5</v>
+      </c>
+      <c r="B21">
+        <v>2.5</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>-0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix error in topology file generation
</commit_message>
<xml_diff>
--- a/Final Project/topo_tool.xlsx
+++ b/Final Project/topo_tool.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9576" windowHeight="2028" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9570" windowHeight="2025" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Bonds" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="Coords" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,12 +31,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="19">
   <si>
     <t>outputFile.write(f"{9*i +</t>
-  </si>
-  <si>
-    <t>outputFile.write(f'{13*i +</t>
-  </si>
-  <si>
-    <t>outputFile.write(f'{12*i +</t>
   </si>
   <si>
     <t>C</t>
@@ -110,6 +103,12 @@
       </rPr>
       <t>specify shift</t>
     </r>
+  </si>
+  <si>
+    <t>outputFile.write(f'{9*i +</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            outputFile.write(f'{9*i +</t>
   </si>
 </sst>
 </file>
@@ -529,14 +528,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -557,7 +556,7 @@
         <v>outputFile.write(f"{9*i +1} {9*i + 0} 2845.12 1.09 \n' )</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -578,7 +577,7 @@
         <v>outputFile.write(f"{9*i +2} {9*i + 0} 2845.12 1.09 \n' )</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -599,7 +598,7 @@
         <v>outputFile.write(f"{9*i +3} {9*i + 0} 2845.12 1.09 \n' )</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -620,7 +619,7 @@
         <v>outputFile.write(f"{9*i +0} {9*i + 4} 2242.624 1.529 \n' )</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -641,7 +640,7 @@
         <v>outputFile.write(f"{9*i +5} {9*i + 4} 2845.12 1.09 \n' )</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -662,7 +661,7 @@
         <v>outputFile.write(f"{9*i +6} {9*i + 4} 2845.12 1.09 \n' )</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -683,7 +682,7 @@
         <v>outputFile.write(f"{9*i +4} {9*i + 7} 2677.76 1.41 \n' )</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -713,19 +712,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="2" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="60.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="64.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -743,13 +744,13 @@
         <v>1.89368</v>
       </c>
       <c r="G1" t="str">
-        <f>CONCATENATE(A1,B1,"} {13*i + ",C1,"} {13*i + ",D1,"} ",E1," ",F1," \n' )")</f>
-        <v>outputFile.write(f'{13*i +1} {13*i + 0} {13*i + 4} 292.88 1.89368 \n' )</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" ref="G1:G4" si="0">CONCATENATE(A1,B1,"} {9*i + ",C1,"} {9*i + ",D1,"} ",E1," ",F1," \n' )")</f>
+        <v>outputFile.write(f'{9*i +1} {9*i + 0} {9*i + 4} 292.88 1.89368 \n' )</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -767,13 +768,13 @@
         <v>1.89368</v>
       </c>
       <c r="G2" t="str">
-        <f t="shared" ref="G2:G13" si="0">CONCATENATE(A2,B2,"} {13*i + ",C2,"} {13*i + ",D2,"} ",E2," ",F2," \n' )")</f>
-        <v>outputFile.write(f'{13*i +2} {13*i + 0} {13*i + 4} 292.88 1.89368 \n' )</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            outputFile.write(f'{9*i +2} {9*i + 0} {9*i + 4} 292.88 1.89368 \n' )</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -792,12 +793,12 @@
       </c>
       <c r="G3" t="str">
         <f t="shared" si="0"/>
-        <v>outputFile.write(f'{13*i +3} {13*i + 0} {13*i + 4} 292.88 1.89368 \n' )</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v xml:space="preserve">            outputFile.write(f'{9*i +3} {9*i + 0} {9*i + 4} 292.88 1.89368 \n' )</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -816,12 +817,12 @@
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
-        <v>outputFile.write(f'{13*i +3} {13*i + 0} {13*i + 2} 276.144 1.88146 \n' )</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v xml:space="preserve">            outputFile.write(f'{9*i +3} {9*i + 0} {9*i + 2} 276.144 1.88146 \n' )</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -839,13 +840,13 @@
         <v>1.8814599999999999</v>
       </c>
       <c r="G5" t="str">
-        <f t="shared" si="0"/>
-        <v>outputFile.write(f'{13*i +3} {13*i + 0} {13*i + 1} 276.144 1.88146 \n' )</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <f>CONCATENATE(A5,B5,"} {9*i + ",C5,"} {9*i + ",D5,"} ",E5," ",F5," \n' )")</f>
+        <v xml:space="preserve">            outputFile.write(f'{9*i +3} {9*i + 0} {9*i + 1} 276.144 1.88146 \n' )</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -863,13 +864,13 @@
         <v>1.8814599999999999</v>
       </c>
       <c r="G6" t="str">
-        <f t="shared" si="0"/>
-        <v>outputFile.write(f'{13*i +2} {13*i + 0} {13*i + 1} 276.144 1.88146 \n' )</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" ref="G6:G13" si="1">CONCATENATE(A6,B6,"} {9*i + ",C6,"} {9*i + ",D6,"} ",E6," ",F6," \n' )")</f>
+        <v xml:space="preserve">            outputFile.write(f'{9*i +2} {9*i + 0} {9*i + 1} 276.144 1.88146 \n' )</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -887,13 +888,13 @@
         <v>1.8814599999999999</v>
       </c>
       <c r="G7" t="str">
-        <f t="shared" si="0"/>
-        <v>outputFile.write(f'{13*i +5} {13*i + 4} {13*i + 6} 276.144 1.88146 \n' )</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">            outputFile.write(f'{9*i +5} {9*i + 4} {9*i + 6} 276.144 1.88146 \n' )</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -911,13 +912,13 @@
         <v>1.93208</v>
       </c>
       <c r="G8" t="str">
-        <f t="shared" si="0"/>
-        <v>outputFile.write(f'{13*i +0} {13*i + 4} {13*i + 6} 313.8 1.93208 \n' )</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">            outputFile.write(f'{9*i +0} {9*i + 4} {9*i + 6} 313.8 1.93208 \n' )</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -935,13 +936,13 @@
         <v>1.93208</v>
       </c>
       <c r="G9" t="str">
-        <f t="shared" si="0"/>
-        <v>outputFile.write(f'{13*i +0} {13*i + 4} {13*i + 5} 313.8 1.93208 \n' )</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">            outputFile.write(f'{9*i +0} {9*i + 4} {9*i + 5} 313.8 1.93208 \n' )</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -959,13 +960,13 @@
         <v>1.9111400000000001</v>
       </c>
       <c r="G10" t="str">
-        <f t="shared" si="0"/>
-        <v>outputFile.write(f'{13*i +0} {13*i + 4} {13*i + 7} 414.4 1.91114 \n' )</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">            outputFile.write(f'{9*i +0} {9*i + 4} {9*i + 7} 414.4 1.91114 \n' )</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B11">
         <v>4</v>
@@ -983,13 +984,13 @@
         <v>1.89368</v>
       </c>
       <c r="G11" t="str">
-        <f t="shared" si="0"/>
-        <v>outputFile.write(f'{13*i +4} {13*i + 7} {13*i + 8} 460.24 1.89368 \n' )</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">            outputFile.write(f'{9*i +4} {9*i + 7} {9*i + 8} 460.24 1.89368 \n' )</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B12">
         <v>5</v>
@@ -1007,13 +1008,13 @@
         <v>1.9111400000000001</v>
       </c>
       <c r="G12" t="str">
-        <f t="shared" si="0"/>
-        <v>outputFile.write(f'{13*i +5} {13*i + 4} {13*i + 7} 292.88 1.91114 \n' )</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">            outputFile.write(f'{9*i +5} {9*i + 4} {9*i + 7} 292.88 1.91114 \n' )</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B13">
         <v>6</v>
@@ -1031,8 +1032,8 @@
         <v>1.9111400000000001</v>
       </c>
       <c r="G13" t="str">
-        <f t="shared" si="0"/>
-        <v>outputFile.write(f'{13*i +6} {13*i + 4} {13*i + 7} 292.88 1.91114 \n' )</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">            outputFile.write(f'{9*i +6} {9*i + 4} {9*i + 7} 292.88 1.91114 \n' )</v>
       </c>
     </row>
   </sheetData>
@@ -1044,20 +1045,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="2" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="84.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="84.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -1084,13 +1087,13 @@
         <v>-3.91622</v>
       </c>
       <c r="J1" t="str">
-        <f>CONCATENATE(A1,B1,"} {12*i + ",C1,"} {12*i + ",D1,"} {12*i + ",E1,"} ",F1," ",G1," ",H1," ",I1," \n' )")</f>
-        <v>outputFile.write(f'{12*i +1} {12*i + 0} {12*i + 4} {12*i + 5} 0.6276 1.8828 0 -3.91622 \n' )</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+        <f>CONCATENATE(A1,B1,"} {9*i + ",C1,"} {9*i + ",D1,"} {9*i + ",E1,"} ",F1," ",G1," ",H1," ",I1," \n' )")</f>
+        <v>outputFile.write(f'{9*i +1} {9*i + 0} {9*i + 4} {9*i + 5} 0.6276 1.8828 0 -3.91622 \n' )</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -1117,13 +1120,13 @@
         <v>-3.91622</v>
       </c>
       <c r="J2" t="str">
-        <f t="shared" ref="J2:J12" si="0">CONCATENATE(A2,B2,"} {12*i + ",C2,"} {12*i + ",D2,"} {12*i + ",E2,"} ",F2," ",G2," ",H2," ",I2," \n' )")</f>
-        <v>outputFile.write(f'{12*i +2} {12*i + 0} {12*i + 4} {12*i + 5} 0.6276 1.8828 0 -3.91622 \n' )</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+        <f t="shared" ref="J2:J12" si="0">CONCATENATE(A2,B2,"} {9*i + ",C2,"} {9*i + ",D2,"} {9*i + ",E2,"} ",F2," ",G2," ",H2," ",I2," \n' )")</f>
+        <v xml:space="preserve">            outputFile.write(f'{9*i +2} {9*i + 0} {9*i + 4} {9*i + 5} 0.6276 1.8828 0 -3.91622 \n' )</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -1151,12 +1154,12 @@
       </c>
       <c r="J3" t="str">
         <f t="shared" si="0"/>
-        <v>outputFile.write(f'{12*i +3} {12*i + 0} {12*i + 4} {12*i + 5} 0.6276 1.8828 0 -3.91622 \n' )</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+        <v xml:space="preserve">            outputFile.write(f'{9*i +3} {9*i + 0} {9*i + 4} {9*i + 5} 0.6276 1.8828 0 -3.91622 \n' )</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1184,12 +1187,12 @@
       </c>
       <c r="J4" t="str">
         <f t="shared" si="0"/>
-        <v>outputFile.write(f'{12*i +1} {12*i + 0} {12*i + 4} {12*i + 6} 0.6276 1.8828 0 -3.91622 \n' )</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+        <v xml:space="preserve">            outputFile.write(f'{9*i +1} {9*i + 0} {9*i + 4} {9*i + 6} 0.6276 1.8828 0 -3.91622 \n' )</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -1217,12 +1220,12 @@
       </c>
       <c r="J5" t="str">
         <f t="shared" si="0"/>
-        <v>outputFile.write(f'{12*i +2} {12*i + 0} {12*i + 4} {12*i + 6} 0.6276 1.8828 0 -3.91622 \n' )</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+        <v xml:space="preserve">            outputFile.write(f'{9*i +2} {9*i + 0} {9*i + 4} {9*i + 6} 0.6276 1.8828 0 -3.91622 \n' )</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B6">
         <v>3</v>
@@ -1250,12 +1253,12 @@
       </c>
       <c r="J6" t="str">
         <f t="shared" si="0"/>
-        <v>outputFile.write(f'{12*i +3} {12*i + 0} {12*i + 4} {12*i + 6} 0.6276 1.8828 0 -3.91622 \n' )</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <v xml:space="preserve">            outputFile.write(f'{9*i +3} {9*i + 0} {9*i + 4} {9*i + 6} 0.6276 1.8828 0 -3.91622 \n' )</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1283,12 +1286,12 @@
       </c>
       <c r="J7" t="str">
         <f t="shared" si="0"/>
-        <v>outputFile.write(f'{12*i +1} {12*i + 0} {12*i + 4} {12*i + 7} 0.97905 2.93716 0 -3.91622 \n' )</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <v xml:space="preserve">            outputFile.write(f'{9*i +1} {9*i + 0} {9*i + 4} {9*i + 7} 0.97905 2.93716 0 -3.91622 \n' )</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -1316,12 +1319,12 @@
       </c>
       <c r="J8" t="str">
         <f t="shared" si="0"/>
-        <v>outputFile.write(f'{12*i +2} {12*i + 0} {12*i + 4} {12*i + 7} 0.97905 2.93716 0 -3.91622 \n' )</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+        <v xml:space="preserve">            outputFile.write(f'{9*i +2} {9*i + 0} {9*i + 4} {9*i + 7} 0.97905 2.93716 0 -3.91622 \n' )</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -1349,12 +1352,12 @@
       </c>
       <c r="J9" t="str">
         <f t="shared" si="0"/>
-        <v>outputFile.write(f'{12*i +3} {12*i + 0} {12*i + 4} {12*i + 7} 0.97905 2.93716 0 -3.91622 \n' )</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+        <v xml:space="preserve">            outputFile.write(f'{9*i +3} {9*i + 0} {9*i + 4} {9*i + 7} 0.97905 2.93716 0 -3.91622 \n' )</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -1382,12 +1385,12 @@
       </c>
       <c r="J10" t="str">
         <f t="shared" si="0"/>
-        <v>outputFile.write(f'{12*i +0} {12*i + 4} {12*i + 7} {12*i + 8} -0.4431 3.83255 0.72801 -4.11705 \n' )</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+        <v xml:space="preserve">            outputFile.write(f'{9*i +0} {9*i + 4} {9*i + 7} {9*i + 8} -0.4431 3.83255 0.72801 -4.11705 \n' )</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B11">
         <v>5</v>
@@ -1415,12 +1418,12 @@
       </c>
       <c r="J11" t="str">
         <f t="shared" si="0"/>
-        <v>outputFile.write(f'{12*i +5} {12*i + 4} {12*i + 7} {12*i + 8} 0.9414 2.8242 0 -3.7656 \n' )</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+        <v xml:space="preserve">            outputFile.write(f'{9*i +5} {9*i + 4} {9*i + 7} {9*i + 8} 0.9414 2.8242 0 -3.7656 \n' )</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B12">
         <v>6</v>
@@ -1448,7 +1451,7 @@
       </c>
       <c r="J12" t="str">
         <f t="shared" si="0"/>
-        <v>outputFile.write(f'{12*i +6} {12*i + 4} {12*i + 7} {12*i + 8} 0.9414 2.8242 0 -3.7656 \n' )</v>
+        <v xml:space="preserve">            outputFile.write(f'{9*i +6} {9*i + 4} {9*i + 7} {9*i + 8} 0.9414 2.8242 0 -3.7656 \n' )</v>
       </c>
     </row>
   </sheetData>
@@ -1464,12 +1467,12 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>3.5</v>
       </c>
@@ -1481,7 +1484,7 @@
         <v>outputFile.write('3.5 0.276144 \n')</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2.5</v>
       </c>
@@ -1493,7 +1496,7 @@
         <v>outputFile.write('2.5 0.12552 \n')</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2.5</v>
       </c>
@@ -1505,7 +1508,7 @@
         <v>outputFile.write('2.5 0.12552 \n')</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2.5</v>
       </c>
@@ -1517,7 +1520,7 @@
         <v>outputFile.write('2.5 0.12552 \n')</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3.5</v>
       </c>
@@ -1529,7 +1532,7 @@
         <v>outputFile.write('3.5 0.276144 \n')</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2.5</v>
       </c>
@@ -1541,7 +1544,7 @@
         <v>outputFile.write('2.5 0.12552 \n')</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2.5</v>
       </c>
@@ -1553,7 +1556,7 @@
         <v>outputFile.write('2.5 0.12552 \n')</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3.12</v>
       </c>
@@ -1565,7 +1568,7 @@
         <v>outputFile.write('3.12 0.71128 \n')</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -1577,7 +1580,7 @@
         <v>outputFile.write('0 0 \n')</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4166</v>
       </c>
@@ -1586,7 +1589,7 @@
         <v>899.85599999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1284</v>
       </c>
@@ -1595,7 +1598,7 @@
         <v>277.34399999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>3488</v>
       </c>
@@ -1604,7 +1607,7 @@
         <v>753.40800000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>228</v>
       </c>
@@ -1622,15 +1625,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B1">
         <f>M24</f>
@@ -1649,9 +1652,9 @@
         <v>outputFile.write(f'C {rand[i][0] + -0.95} {rand[i][1] + 0.95} {rand[i][2] + 0.777817459305202} \n')</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <f t="shared" ref="B2:B9" si="1">M25</f>
@@ -1670,9 +1673,9 @@
         <v xml:space="preserve">            outputFile.write(f'H {rand[i][0] + -1.80710678118655} {rand[i][1] + 0.392893218813452} {rand[i][2] + 0.565685424949238} \n')</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <f t="shared" si="1"/>
@@ -1691,9 +1694,9 @@
         <v xml:space="preserve">            outputFile.write(f'H {rand[i][0] + -1.15} {rand[i][1] + 1.15} {rand[i][2] + 1.90918830920368} \n')</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <f t="shared" si="1"/>
@@ -1712,9 +1715,9 @@
         <v xml:space="preserve">            outputFile.write(f'H {rand[i][0] + -0.442893218813453} {rand[i][1] + 1.85710678118655} {rand[i][2] + 0.494974746830583} \n')</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B5">
         <f t="shared" si="1"/>
@@ -1733,9 +1736,9 @@
         <v xml:space="preserve">            outputFile.write(f'C {rand[i][0] + 0} {rand[i][1] + 0} {rand[i][2] + 0} \n')</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B6">
         <f t="shared" si="1"/>
@@ -1754,9 +1757,9 @@
         <v xml:space="preserve">            outputFile.write(f'H {rand[i][0] + 0.965685424949238} {rand[i][1] + 0.165685424949238} {rand[i][2] + 0.565685424949238} \n')</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B7">
         <f t="shared" si="1"/>
@@ -1775,9 +1778,9 @@
         <v xml:space="preserve">            outputFile.write(f'H {rand[i][0] + -0.0949747468305832} {rand[i][1] + -0.894974746830583} {rand[i][2] + 0.565685424949238} \n')</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B8">
         <f t="shared" si="1"/>
@@ -1796,9 +1799,9 @@
         <v xml:space="preserve">            outputFile.write(f'O {rand[i][0] + 0.5} {rand[i][1] + -0.5} {rand[i][2] + -1.41421356237309} \n')</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B9">
         <f t="shared" si="1"/>
@@ -1817,23 +1820,23 @@
         <v xml:space="preserve">            outputFile.write(f'H {rand[i][0] + 1.00355339059327} {rand[i][1] + -0.296446609406726} {rand[i][2] + -1.90918830920368} \n')</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1848,7 +1851,7 @@
         <v>-3.5</v>
       </c>
       <c r="F13">
-        <f t="shared" ref="F13:G21" si="3">-B$17</f>
+        <f t="shared" ref="F13:G13" si="3">-B$17</f>
         <v>-2</v>
       </c>
       <c r="G13">
@@ -1868,7 +1871,7 @@
         <v>-0.4</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
@@ -1891,7 +1894,7 @@
         <v>-0.7</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1914,7 +1917,7 @@
         <v>0.20000000000000007</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1937,7 +1940,7 @@
         <v>-0.8</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3.5</v>
       </c>
@@ -1960,10 +1963,10 @@
         <v>0</v>
       </c>
       <c r="L17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3.5</v>
       </c>
@@ -1986,7 +1989,7 @@
         <v>0.79999999999999993</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>3.5</v>
       </c>
@@ -2009,7 +2012,7 @@
         <v>0.79999999999999993</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>5</v>
       </c>
@@ -2032,7 +2035,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>5.5</v>
       </c>
@@ -2055,12 +2058,12 @@
         <v>-0.7</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>1</v>
       </c>
@@ -2101,7 +2104,7 @@
         <v>0.77781745930520207</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>0</v>
       </c>
@@ -2141,7 +2144,7 @@
         <v>0.5656854249492379</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>0</v>
       </c>
@@ -2181,7 +2184,7 @@
         <v>1.9091883092036781</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
@@ -2213,9 +2216,9 @@
         <v>0.49497474683058307</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B28" s="6"/>
       <c r="C28" s="7"/>
@@ -2247,9 +2250,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B29" s="9">
         <v>0</v>
@@ -2283,7 +2286,7 @@
         <v>0.56568542494923801</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E30">
         <v>0</v>
       </c>
@@ -2312,7 +2315,7 @@
         <v>0.56568542494923801</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E31">
         <v>1.5</v>
       </c>
@@ -2341,7 +2344,7 @@
         <v>-1.4142135623730949</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <f>COS(B37)</f>
         <v>0.70710678118654757</v>
@@ -2381,7 +2384,7 @@
         <v>-1.9091883092036781</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>0</v>
       </c>
@@ -2392,16 +2395,16 @@
         <v>0</v>
       </c>
       <c r="E33" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I33" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="M33" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <f>-SIN(B37)</f>
         <v>0.70710678118654746</v>
@@ -2414,21 +2417,21 @@
         <v>0.70710678118654757</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="6"/>
       <c r="C35" s="7"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="7"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B37" s="9">
         <f>-PI()/4</f>
@@ -2436,7 +2439,7 @@
       </c>
       <c r="C37" s="10"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <f>COS(B45)</f>
         <v>0.70710678118654757</v>
@@ -2449,7 +2452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <f>SIN(B45)</f>
         <v>0.70710678118654746</v>
@@ -2462,7 +2465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>0</v>
       </c>
@@ -2473,21 +2476,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="B43" s="6"/>
       <c r="C43" s="7"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B44" s="6"/>
       <c r="C44" s="7"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B45" s="9">
         <f>PI()/4</f>

</xml_diff>